<commit_message>
Fixed codebook for new PS
</commit_message>
<xml_diff>
--- a/PDS/Datasets/gss_codebook.xlsx
+++ b/PDS/Datasets/gss_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c54237df8f2edc7e/Spring2020/Political Data Science/Problem Sets/PS 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c54237df8f2edc7e/Documents/GitHub/jmontgomery.github.io/PDS/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="8_{A28BE22B-D4B2-40A7-A547-790B2F7E610F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CBE6294F-1DCC-48C5-A7AB-D9BEAB578D08}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19455" windowHeight="13875" xr2:uid="{1F8A5C0C-F8CB-485F-9688-384FE2ED1421}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19666" windowHeight="13875" xr2:uid="{1F8A5C0C-F8CB-485F-9688-384FE2ED1421}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727921B4-B9AF-4077-8EA9-67B9F2981B4F}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>